<commit_message>
Bug fixes on reports & dashboard
</commit_message>
<xml_diff>
--- a/public/reportTemplates/ContributionReportTemplate.xlsx
+++ b/public/reportTemplates/ContributionReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zelalemg/Desktop/EHIA/CBHI/cbhi-enrollment-app/public/reportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D9D6E8-4C7C-3846-BDD2-030F8E2CFC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6AD864-7C2B-3F4B-97EB-03E670DAFF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="980" windowWidth="27640" windowHeight="15500" xr2:uid="{C86269E4-111D-9C4C-8B60-B3FD0A26D3A1}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Woreda</t>
   </si>
   <si>
-    <t xml:space="preserve">Total Contribution collected from paying members </t>
-  </si>
-  <si>
     <t>General Subsidy</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>${totalSubsidy}</t>
+  </si>
+  <si>
+    <t>Total Contribution collected from paying members</t>
   </si>
 </sst>
 </file>
@@ -752,6 +752,9 @@
   <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -810,52 +813,39 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="3" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="3" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="4" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="11" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -886,27 +876,21 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -940,23 +924,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1282,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097A6F85-3A1F-4A48-B820-9E7BBA08DE04}">
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -1368,66 +1347,66 @@
         <v>5</v>
       </c>
       <c r="B4" s="56"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="41"/>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="50" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="50"/>
       <c r="L4" s="51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="51"/>
       <c r="N4" s="51"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:29" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="57" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="58"/>
-      <c r="C5" s="7"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="59"/>
       <c r="F5" s="59"/>
       <c r="G5" s="59"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="8"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:29" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="14"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="15"/>
     </row>
     <row r="7" spans="1:29" ht="4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38"/>
@@ -1456,17 +1435,17 @@
       <c r="D8" s="63"/>
       <c r="E8" s="64"/>
       <c r="F8" s="60" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="G8" s="61"/>
       <c r="H8" s="61"/>
       <c r="I8" s="61"/>
       <c r="J8" s="61"/>
       <c r="K8" s="46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L8" s="48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M8" s="49"/>
       <c r="N8" s="49"/>
@@ -1474,101 +1453,101 @@
         <v>4</v>
       </c>
       <c r="P8" s="42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="37" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="C9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="E9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="F9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="I9" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="J9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="21" t="s">
-        <v>26</v>
-      </c>
       <c r="K9" s="47"/>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="N9" s="23" t="s">
+      <c r="N9" s="24" t="s">
         <v>6</v>
       </c>
       <c r="O9" s="45"/>
       <c r="P9" s="43"/>
     </row>
     <row r="10" spans="1:29" ht="73" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="C10" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="D10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="E10" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="F10" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="G10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="H10" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="I10" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="J10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="29" t="s">
+      <c r="K10" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="L10" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="M10" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="N10" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="N10" s="30" t="s">
+      <c r="O10" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="30" t="s">
+      <c r="P10" s="32" t="s">
         <v>41</v>
-      </c>
-      <c r="P10" s="31" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -1591,7 +1570,7 @@
     </row>
     <row r="12" spans="1:29" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="53"/>
       <c r="C12" s="53"/>
@@ -1608,22 +1587,22 @@
       <c r="N12" s="53"/>
       <c r="O12" s="53"/>
       <c r="P12" s="54"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="32"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="32"/>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="32"/>
-      <c r="AC12" s="32"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="72ZFXlH/uf1gG7Mo+X3YtB5uXPC4KTMnEY305007OH0C1xdW0k/Mdtmr+S+3l3jsZ8A+J3gvrjqWr3LPfMFe0Q==" saltValue="n2Eel10JuWKtQfcL4BnCNA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="gAqye/Tq504yarGm5zJicvk1XKYgaeBL8JTspFp2DZFjLUgIyYccTpBnv2HhJ5wf6cZXARdZb8EfrYPp85KTmw==" saltValue="XQwf40RfjVrYHqqDoha3xA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0"/>
   <mergeCells count="16">
     <mergeCell ref="A12:P12"/>
     <mergeCell ref="A4:B4"/>

</xml_diff>